<commit_message>
big simple importer update incl. sync with All-In-One-Importer
</commit_message>
<xml_diff>
--- a/de.bund.bfr.knime.openkrise.db/src/de/bund/bfr/knime/openkrise/db/imports/custom/bfrnewformat/FCL_Uptrace_Prod_simple_en.xlsx
+++ b/de.bund.bfr.knime.openkrise.db/src/de/bund/bfr/knime/openkrise/db/imports/custom/bfrnewformat/FCL_Uptrace_Prod_simple_en.xlsx
@@ -603,7 +603,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="52">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -987,21 +987,6 @@
       </top>
       <bottom style="medium">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1375,7 +1360,7 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="32" fillId="29" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="8" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
@@ -1439,53 +1424,26 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1499,14 +1457,10 @@
     <xf numFmtId="49" fontId="8" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -1525,15 +1479,125 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="1" fontId="7" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="6" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="6" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="5" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="5" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="5" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="36" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="36" fillId="3" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1543,6 +1607,10 @@
     <xf numFmtId="1" fontId="3" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="34" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="34" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -1551,57 +1619,6 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="34" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="5" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="5" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="5" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="36" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="36" fillId="3" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1617,70 +1634,7 @@
     <xf numFmtId="1" fontId="3" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="6" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="5" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="33" fillId="5" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -2098,31 +2052,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S102"/>
+  <dimension ref="A1:M102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="19.73046875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="25.86328125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="12.3984375" style="6" customWidth="1"/>
     <col min="4" max="4" width="16" style="6" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" style="12" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="12" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="16.265625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="7.265625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="7.73046875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="9.1328125" style="12" customWidth="1"/>
     <col min="9" max="9" width="22" style="6" customWidth="1"/>
-    <col min="10" max="10" width="21.28515625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="21.265625" style="6" customWidth="1"/>
     <col min="11" max="11" width="40" style="6" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" style="6" customWidth="1"/>
-    <col min="13" max="13" width="19.28515625" style="6" customWidth="1"/>
-    <col min="14" max="14" width="27" style="29" customWidth="1"/>
-    <col min="15" max="18" width="11.42578125" style="29"/>
-    <col min="19" max="16384" width="11.42578125" style="6"/>
+    <col min="12" max="12" width="13.265625" style="6" customWidth="1"/>
+    <col min="13" max="13" width="19.265625" style="6" customWidth="1"/>
+    <col min="14" max="16384" width="11.3984375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="23" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="21" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="16" t="s">
         <v>3</v>
       </c>
@@ -2138,132 +2090,113 @@
       <c r="E1" s="18"/>
       <c r="F1" s="19"/>
       <c r="G1" s="20"/>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="21"/>
-    </row>
-    <row r="2" spans="1:19" s="23" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="21"/>
-    </row>
-    <row r="3" spans="1:19" s="7" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="78" t="s">
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="79"/>
+    </row>
+    <row r="2" spans="1:13" s="21" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="25"/>
+    </row>
+    <row r="3" spans="1:13" s="7" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="79"/>
-      <c r="L3" s="79"/>
-      <c r="M3" s="80"/>
-      <c r="N3" s="34"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-    </row>
-    <row r="4" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="76" t="s">
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="53"/>
+    </row>
+    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="90" t="s">
+      <c r="B4" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="91"/>
-      <c r="D4" s="90" t="s">
+      <c r="C4" s="64"/>
+      <c r="D4" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="91"/>
-      <c r="F4" s="73" t="s">
+      <c r="E4" s="64"/>
+      <c r="F4" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="84" t="s">
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="85"/>
-      <c r="L4" s="86"/>
-      <c r="M4" s="61" t="s">
+      <c r="K4" s="58"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="N4" s="35"/>
-    </row>
-    <row r="5" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="76"/>
-      <c r="B5" s="71" t="s">
+    </row>
+    <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="43"/>
+      <c r="B5" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="71" t="s">
+      <c r="C5" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="71" t="s">
+      <c r="D5" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="71" t="s">
+      <c r="E5" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="73" t="s">
+      <c r="F5" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="74"/>
-      <c r="H5" s="75"/>
-      <c r="I5" s="71" t="s">
+      <c r="G5" s="86"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="94" t="s">
+      <c r="J5" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="94" t="s">
+      <c r="K5" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="94" t="s">
+      <c r="L5" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="M5" s="62"/>
-      <c r="N5" s="34"/>
-    </row>
-    <row r="6" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="96"/>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
+      <c r="M5" s="71"/>
+    </row>
+    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="69"/>
+      <c r="B6" s="84"/>
+      <c r="C6" s="84"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="84"/>
       <c r="F6" s="15" t="s">
         <v>12</v>
       </c>
@@ -2273,277 +2206,228 @@
       <c r="H6" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="72"/>
-      <c r="J6" s="95"/>
-      <c r="K6" s="95"/>
-      <c r="L6" s="95"/>
-      <c r="M6" s="97"/>
-      <c r="N6" s="34"/>
-    </row>
-    <row r="7" spans="1:19" s="7" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
+      <c r="I6" s="84"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="68"/>
+      <c r="L6" s="68"/>
+      <c r="M6" s="88"/>
+    </row>
+    <row r="7" spans="1:13" s="7" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="40"/>
-      <c r="M7" s="41"/>
-      <c r="N7" s="34"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="29"/>
-    </row>
-    <row r="8" spans="1:19" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="55" t="s">
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="33"/>
+    </row>
+    <row r="8" spans="1:13" s="27" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="56"/>
-      <c r="J8" s="56"/>
-      <c r="K8" s="56"/>
-      <c r="L8" s="56"/>
-      <c r="M8" s="57"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="31"/>
-      <c r="R8" s="31"/>
-      <c r="S8" s="32"/>
-    </row>
-    <row r="9" spans="1:19" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="58" t="s">
+      <c r="B8" s="81"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="81"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="81"/>
+      <c r="K8" s="81"/>
+      <c r="L8" s="81"/>
+      <c r="M8" s="82"/>
+    </row>
+    <row r="9" spans="1:13" s="27" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="59"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
-      <c r="H9" s="59"/>
-      <c r="I9" s="59"/>
-      <c r="J9" s="59"/>
-      <c r="K9" s="59"/>
-      <c r="L9" s="59"/>
-      <c r="M9" s="60"/>
-      <c r="N9" s="31"/>
-      <c r="O9" s="31"/>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="32"/>
-    </row>
-    <row r="10" spans="1:19" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="58" t="s">
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="49"/>
+      <c r="M9" s="50"/>
+    </row>
+    <row r="10" spans="1:13" s="27" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="59"/>
-      <c r="L10" s="59"/>
-      <c r="M10" s="60"/>
-      <c r="N10" s="31"/>
-      <c r="O10" s="31"/>
-      <c r="P10" s="31"/>
-      <c r="Q10" s="31"/>
-      <c r="R10" s="31"/>
-      <c r="S10" s="32"/>
-    </row>
-    <row r="11" spans="1:19" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="58" t="s">
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="49"/>
+      <c r="M10" s="50"/>
+    </row>
+    <row r="11" spans="1:13" s="27" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="59"/>
-      <c r="H11" s="59"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="59"/>
-      <c r="K11" s="59"/>
-      <c r="L11" s="59"/>
-      <c r="M11" s="60"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="31"/>
-      <c r="Q11" s="31"/>
-      <c r="R11" s="31"/>
-      <c r="S11" s="32"/>
-    </row>
-    <row r="12" spans="1:19" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="58" t="s">
+      <c r="B11" s="49"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="50"/>
+    </row>
+    <row r="12" spans="1:13" s="27" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="59"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="59"/>
-      <c r="I12" s="59"/>
-      <c r="J12" s="59"/>
-      <c r="K12" s="59"/>
-      <c r="L12" s="59"/>
-      <c r="M12" s="60"/>
-      <c r="N12" s="31"/>
-      <c r="O12" s="31"/>
-      <c r="P12" s="31"/>
-      <c r="Q12" s="31"/>
-      <c r="R12" s="31"/>
-      <c r="S12" s="32"/>
-    </row>
-    <row r="13" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="81" t="s">
+      <c r="B12" s="49"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="49"/>
+      <c r="M12" s="50"/>
+    </row>
+    <row r="13" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="82"/>
-      <c r="C13" s="82"/>
-      <c r="D13" s="82"/>
-      <c r="E13" s="82"/>
-      <c r="F13" s="82"/>
-      <c r="G13" s="82"/>
-      <c r="H13" s="82"/>
-      <c r="I13" s="82"/>
-      <c r="J13" s="82"/>
-      <c r="K13" s="82"/>
-      <c r="L13" s="82"/>
-      <c r="M13" s="83"/>
-      <c r="N13" s="34"/>
-    </row>
-    <row r="14" spans="1:19" s="9" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="76" t="s">
+      <c r="B13" s="55"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="55"/>
+      <c r="K13" s="55"/>
+      <c r="L13" s="55"/>
+      <c r="M13" s="56"/>
+    </row>
+    <row r="14" spans="1:13" s="9" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="92" t="s">
+      <c r="B14" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="93"/>
-      <c r="D14" s="92" t="s">
+      <c r="C14" s="66"/>
+      <c r="D14" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="93"/>
-      <c r="F14" s="66" t="s">
+      <c r="E14" s="66"/>
+      <c r="F14" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="67"/>
-      <c r="H14" s="67"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="87" t="s">
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="K14" s="88"/>
-      <c r="L14" s="89"/>
-      <c r="M14" s="61" t="s">
+      <c r="K14" s="61"/>
+      <c r="L14" s="62"/>
+      <c r="M14" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="N14" s="42"/>
-      <c r="O14" s="30"/>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="30"/>
-      <c r="R14" s="30"/>
-    </row>
-    <row r="15" spans="1:19" s="9" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="76"/>
-      <c r="B15" s="64" t="s">
+    </row>
+    <row r="15" spans="1:13" s="9" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="43"/>
+      <c r="B15" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="64" t="s">
+      <c r="C15" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="64" t="s">
+      <c r="D15" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="64" t="s">
+      <c r="E15" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="66" t="s">
+      <c r="F15" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="67"/>
-      <c r="H15" s="68"/>
-      <c r="I15" s="64" t="s">
+      <c r="G15" s="46"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="J15" s="69" t="s">
+      <c r="J15" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="K15" s="69" t="s">
+      <c r="K15" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="L15" s="69" t="s">
+      <c r="L15" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="M15" s="62"/>
-      <c r="N15" s="42"/>
-      <c r="O15" s="30"/>
-      <c r="P15" s="30"/>
-      <c r="Q15" s="30"/>
-      <c r="R15" s="30"/>
-    </row>
-    <row r="16" spans="1:19" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="77"/>
-      <c r="B16" s="65"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="51" t="s">
+      <c r="M15" s="71"/>
+    </row>
+    <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="44"/>
+      <c r="B16" s="74"/>
+      <c r="C16" s="74"/>
+      <c r="D16" s="74"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="51" t="s">
+      <c r="G16" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="51" t="s">
+      <c r="H16" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="65"/>
-      <c r="J16" s="70"/>
-      <c r="K16" s="70"/>
-      <c r="L16" s="70"/>
-      <c r="M16" s="63"/>
-      <c r="N16" s="34"/>
-    </row>
-    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="44"/>
-      <c r="B17" s="45"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="45"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="49"/>
-      <c r="L17" s="49"/>
-      <c r="M17" s="50"/>
-      <c r="N17" s="34"/>
-    </row>
-    <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I16" s="74"/>
+      <c r="J16" s="76"/>
+      <c r="K16" s="76"/>
+      <c r="L16" s="76"/>
+      <c r="M16" s="72"/>
+    </row>
+    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="35"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="41"/>
+    </row>
+    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="1"/>
       <c r="C18" s="2"/>
@@ -2554,12 +2438,11 @@
       <c r="H18" s="13"/>
       <c r="I18" s="1"/>
       <c r="J18" s="8"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="43"/>
-      <c r="N18" s="34"/>
-    </row>
-    <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="34"/>
+    </row>
+    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2"/>
@@ -2570,12 +2453,11 @@
       <c r="H19" s="13"/>
       <c r="I19" s="1"/>
       <c r="J19" s="8"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="43"/>
-      <c r="N19" s="34"/>
-    </row>
-    <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="34"/>
+    </row>
+    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="1"/>
       <c r="C20" s="2"/>
@@ -2586,12 +2468,11 @@
       <c r="H20" s="13"/>
       <c r="I20" s="1"/>
       <c r="J20" s="8"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="43"/>
-      <c r="N20" s="34"/>
-    </row>
-    <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="34"/>
+    </row>
+    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="1"/>
       <c r="C21" s="2"/>
@@ -2602,12 +2483,11 @@
       <c r="H21" s="13"/>
       <c r="I21" s="1"/>
       <c r="J21" s="8"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="43"/>
-      <c r="N21" s="34"/>
-    </row>
-    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="34"/>
+    </row>
+    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="1"/>
       <c r="C22" s="2"/>
@@ -2618,12 +2498,11 @@
       <c r="H22" s="13"/>
       <c r="I22" s="1"/>
       <c r="J22" s="8"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="43"/>
-      <c r="N22" s="34"/>
-    </row>
-    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="34"/>
+    </row>
+    <row r="23" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2634,12 +2513,11 @@
       <c r="H23" s="13"/>
       <c r="I23" s="1"/>
       <c r="J23" s="8"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="43"/>
-      <c r="N23" s="34"/>
-    </row>
-    <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="34"/>
+    </row>
+    <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2650,12 +2528,11 @@
       <c r="H24" s="13"/>
       <c r="I24" s="1"/>
       <c r="J24" s="8"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="43"/>
-      <c r="N24" s="34"/>
-    </row>
-    <row r="25" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="34"/>
+    </row>
+    <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2666,12 +2543,11 @@
       <c r="H25" s="13"/>
       <c r="I25" s="1"/>
       <c r="J25" s="8"/>
-      <c r="K25" s="28"/>
-      <c r="L25" s="28"/>
-      <c r="M25" s="43"/>
-      <c r="N25" s="34"/>
-    </row>
-    <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K25" s="26"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="34"/>
+    </row>
+    <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2682,12 +2558,11 @@
       <c r="H26" s="13"/>
       <c r="I26" s="1"/>
       <c r="J26" s="8"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="43"/>
-      <c r="N26" s="34"/>
-    </row>
-    <row r="27" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K26" s="26"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="34"/>
+    </row>
+    <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2698,12 +2573,11 @@
       <c r="H27" s="13"/>
       <c r="I27" s="1"/>
       <c r="J27" s="8"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="43"/>
-      <c r="N27" s="34"/>
-    </row>
-    <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K27" s="26"/>
+      <c r="L27" s="26"/>
+      <c r="M27" s="34"/>
+    </row>
+    <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2714,12 +2588,11 @@
       <c r="H28" s="13"/>
       <c r="I28" s="1"/>
       <c r="J28" s="8"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="43"/>
-      <c r="N28" s="34"/>
-    </row>
-    <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K28" s="26"/>
+      <c r="L28" s="26"/>
+      <c r="M28" s="34"/>
+    </row>
+    <row r="29" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -2730,12 +2603,11 @@
       <c r="H29" s="13"/>
       <c r="I29" s="1"/>
       <c r="J29" s="8"/>
-      <c r="K29" s="28"/>
-      <c r="L29" s="28"/>
-      <c r="M29" s="43"/>
-      <c r="N29" s="34"/>
-    </row>
-    <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K29" s="26"/>
+      <c r="L29" s="26"/>
+      <c r="M29" s="34"/>
+    </row>
+    <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2746,12 +2618,11 @@
       <c r="H30" s="13"/>
       <c r="I30" s="1"/>
       <c r="J30" s="8"/>
-      <c r="K30" s="28"/>
-      <c r="L30" s="28"/>
-      <c r="M30" s="43"/>
-      <c r="N30" s="34"/>
-    </row>
-    <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K30" s="26"/>
+      <c r="L30" s="26"/>
+      <c r="M30" s="34"/>
+    </row>
+    <row r="31" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -2762,12 +2633,11 @@
       <c r="H31" s="13"/>
       <c r="I31" s="1"/>
       <c r="J31" s="8"/>
-      <c r="K31" s="28"/>
-      <c r="L31" s="28"/>
-      <c r="M31" s="43"/>
-      <c r="N31" s="34"/>
-    </row>
-    <row r="32" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K31" s="26"/>
+      <c r="L31" s="26"/>
+      <c r="M31" s="34"/>
+    </row>
+    <row r="32" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -2778,12 +2648,11 @@
       <c r="H32" s="13"/>
       <c r="I32" s="1"/>
       <c r="J32" s="8"/>
-      <c r="K32" s="28"/>
-      <c r="L32" s="28"/>
-      <c r="M32" s="43"/>
-      <c r="N32" s="34"/>
-    </row>
-    <row r="33" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K32" s="26"/>
+      <c r="L32" s="26"/>
+      <c r="M32" s="34"/>
+    </row>
+    <row r="33" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2794,12 +2663,11 @@
       <c r="H33" s="13"/>
       <c r="I33" s="1"/>
       <c r="J33" s="8"/>
-      <c r="K33" s="28"/>
-      <c r="L33" s="28"/>
-      <c r="M33" s="43"/>
-      <c r="N33" s="34"/>
-    </row>
-    <row r="34" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K33" s="26"/>
+      <c r="L33" s="26"/>
+      <c r="M33" s="34"/>
+    </row>
+    <row r="34" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -2810,12 +2678,11 @@
       <c r="H34" s="13"/>
       <c r="I34" s="1"/>
       <c r="J34" s="8"/>
-      <c r="K34" s="28"/>
-      <c r="L34" s="28"/>
-      <c r="M34" s="43"/>
-      <c r="N34" s="34"/>
-    </row>
-    <row r="35" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K34" s="26"/>
+      <c r="L34" s="26"/>
+      <c r="M34" s="34"/>
+    </row>
+    <row r="35" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -2826,12 +2693,11 @@
       <c r="H35" s="13"/>
       <c r="I35" s="1"/>
       <c r="J35" s="8"/>
-      <c r="K35" s="28"/>
-      <c r="L35" s="28"/>
-      <c r="M35" s="43"/>
-      <c r="N35" s="34"/>
-    </row>
-    <row r="36" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K35" s="26"/>
+      <c r="L35" s="26"/>
+      <c r="M35" s="34"/>
+    </row>
+    <row r="36" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2842,12 +2708,11 @@
       <c r="H36" s="13"/>
       <c r="I36" s="1"/>
       <c r="J36" s="8"/>
-      <c r="K36" s="28"/>
-      <c r="L36" s="28"/>
-      <c r="M36" s="43"/>
-      <c r="N36" s="34"/>
-    </row>
-    <row r="37" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K36" s="26"/>
+      <c r="L36" s="26"/>
+      <c r="M36" s="34"/>
+    </row>
+    <row r="37" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -2858,12 +2723,11 @@
       <c r="H37" s="13"/>
       <c r="I37" s="1"/>
       <c r="J37" s="8"/>
-      <c r="K37" s="28"/>
-      <c r="L37" s="28"/>
-      <c r="M37" s="43"/>
-      <c r="N37" s="34"/>
-    </row>
-    <row r="38" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K37" s="26"/>
+      <c r="L37" s="26"/>
+      <c r="M37" s="34"/>
+    </row>
+    <row r="38" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2874,12 +2738,11 @@
       <c r="H38" s="13"/>
       <c r="I38" s="1"/>
       <c r="J38" s="8"/>
-      <c r="K38" s="28"/>
-      <c r="L38" s="28"/>
-      <c r="M38" s="43"/>
-      <c r="N38" s="34"/>
-    </row>
-    <row r="39" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K38" s="26"/>
+      <c r="L38" s="26"/>
+      <c r="M38" s="34"/>
+    </row>
+    <row r="39" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2890,12 +2753,11 @@
       <c r="H39" s="13"/>
       <c r="I39" s="1"/>
       <c r="J39" s="8"/>
-      <c r="K39" s="28"/>
-      <c r="L39" s="28"/>
-      <c r="M39" s="43"/>
-      <c r="N39" s="34"/>
-    </row>
-    <row r="40" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K39" s="26"/>
+      <c r="L39" s="26"/>
+      <c r="M39" s="34"/>
+    </row>
+    <row r="40" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2906,12 +2768,11 @@
       <c r="H40" s="13"/>
       <c r="I40" s="1"/>
       <c r="J40" s="8"/>
-      <c r="K40" s="28"/>
-      <c r="L40" s="28"/>
-      <c r="M40" s="43"/>
-      <c r="N40" s="34"/>
-    </row>
-    <row r="41" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K40" s="26"/>
+      <c r="L40" s="26"/>
+      <c r="M40" s="34"/>
+    </row>
+    <row r="41" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -2922,12 +2783,11 @@
       <c r="H41" s="13"/>
       <c r="I41" s="1"/>
       <c r="J41" s="8"/>
-      <c r="K41" s="28"/>
-      <c r="L41" s="28"/>
-      <c r="M41" s="43"/>
-      <c r="N41" s="34"/>
-    </row>
-    <row r="42" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K41" s="26"/>
+      <c r="L41" s="26"/>
+      <c r="M41" s="34"/>
+    </row>
+    <row r="42" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -2938,12 +2798,11 @@
       <c r="H42" s="13"/>
       <c r="I42" s="1"/>
       <c r="J42" s="8"/>
-      <c r="K42" s="28"/>
-      <c r="L42" s="28"/>
-      <c r="M42" s="43"/>
-      <c r="N42" s="34"/>
-    </row>
-    <row r="43" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K42" s="26"/>
+      <c r="L42" s="26"/>
+      <c r="M42" s="34"/>
+    </row>
+    <row r="43" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -2954,12 +2813,11 @@
       <c r="H43" s="13"/>
       <c r="I43" s="1"/>
       <c r="J43" s="8"/>
-      <c r="K43" s="28"/>
-      <c r="L43" s="28"/>
-      <c r="M43" s="43"/>
-      <c r="N43" s="34"/>
-    </row>
-    <row r="44" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K43" s="26"/>
+      <c r="L43" s="26"/>
+      <c r="M43" s="34"/>
+    </row>
+    <row r="44" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -2970,12 +2828,11 @@
       <c r="H44" s="13"/>
       <c r="I44" s="1"/>
       <c r="J44" s="8"/>
-      <c r="K44" s="28"/>
-      <c r="L44" s="28"/>
-      <c r="M44" s="43"/>
-      <c r="N44" s="34"/>
-    </row>
-    <row r="45" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K44" s="26"/>
+      <c r="L44" s="26"/>
+      <c r="M44" s="34"/>
+    </row>
+    <row r="45" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="3"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -2986,12 +2843,11 @@
       <c r="H45" s="13"/>
       <c r="I45" s="1"/>
       <c r="J45" s="8"/>
-      <c r="K45" s="28"/>
-      <c r="L45" s="28"/>
-      <c r="M45" s="43"/>
-      <c r="N45" s="34"/>
-    </row>
-    <row r="46" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K45" s="26"/>
+      <c r="L45" s="26"/>
+      <c r="M45" s="34"/>
+    </row>
+    <row r="46" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -3002,12 +2858,11 @@
       <c r="H46" s="13"/>
       <c r="I46" s="1"/>
       <c r="J46" s="8"/>
-      <c r="K46" s="28"/>
-      <c r="L46" s="28"/>
-      <c r="M46" s="43"/>
-      <c r="N46" s="34"/>
-    </row>
-    <row r="47" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K46" s="26"/>
+      <c r="L46" s="26"/>
+      <c r="M46" s="34"/>
+    </row>
+    <row r="47" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="3"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -3018,12 +2873,11 @@
       <c r="H47" s="13"/>
       <c r="I47" s="1"/>
       <c r="J47" s="8"/>
-      <c r="K47" s="28"/>
-      <c r="L47" s="28"/>
-      <c r="M47" s="43"/>
-      <c r="N47" s="34"/>
-    </row>
-    <row r="48" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K47" s="26"/>
+      <c r="L47" s="26"/>
+      <c r="M47" s="34"/>
+    </row>
+    <row r="48" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -3034,12 +2888,11 @@
       <c r="H48" s="13"/>
       <c r="I48" s="1"/>
       <c r="J48" s="8"/>
-      <c r="K48" s="28"/>
-      <c r="L48" s="28"/>
-      <c r="M48" s="43"/>
-      <c r="N48" s="34"/>
-    </row>
-    <row r="49" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K48" s="26"/>
+      <c r="L48" s="26"/>
+      <c r="M48" s="34"/>
+    </row>
+    <row r="49" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -3050,12 +2903,11 @@
       <c r="H49" s="13"/>
       <c r="I49" s="1"/>
       <c r="J49" s="8"/>
-      <c r="K49" s="28"/>
-      <c r="L49" s="28"/>
-      <c r="M49" s="43"/>
-      <c r="N49" s="34"/>
-    </row>
-    <row r="50" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K49" s="26"/>
+      <c r="L49" s="26"/>
+      <c r="M49" s="34"/>
+    </row>
+    <row r="50" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="3"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -3066,12 +2918,11 @@
       <c r="H50" s="13"/>
       <c r="I50" s="1"/>
       <c r="J50" s="8"/>
-      <c r="K50" s="28"/>
-      <c r="L50" s="28"/>
-      <c r="M50" s="43"/>
-      <c r="N50" s="34"/>
-    </row>
-    <row r="51" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K50" s="26"/>
+      <c r="L50" s="26"/>
+      <c r="M50" s="34"/>
+    </row>
+    <row r="51" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -3082,12 +2933,11 @@
       <c r="H51" s="13"/>
       <c r="I51" s="1"/>
       <c r="J51" s="8"/>
-      <c r="K51" s="28"/>
-      <c r="L51" s="28"/>
-      <c r="M51" s="43"/>
-      <c r="N51" s="34"/>
-    </row>
-    <row r="52" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K51" s="26"/>
+      <c r="L51" s="26"/>
+      <c r="M51" s="34"/>
+    </row>
+    <row r="52" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -3098,12 +2948,11 @@
       <c r="H52" s="13"/>
       <c r="I52" s="1"/>
       <c r="J52" s="8"/>
-      <c r="K52" s="28"/>
-      <c r="L52" s="28"/>
-      <c r="M52" s="43"/>
-      <c r="N52" s="34"/>
-    </row>
-    <row r="53" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K52" s="26"/>
+      <c r="L52" s="26"/>
+      <c r="M52" s="34"/>
+    </row>
+    <row r="53" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="3"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -3114,12 +2963,11 @@
       <c r="H53" s="13"/>
       <c r="I53" s="1"/>
       <c r="J53" s="8"/>
-      <c r="K53" s="28"/>
-      <c r="L53" s="28"/>
-      <c r="M53" s="43"/>
-      <c r="N53" s="34"/>
-    </row>
-    <row r="54" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K53" s="26"/>
+      <c r="L53" s="26"/>
+      <c r="M53" s="34"/>
+    </row>
+    <row r="54" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="3"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -3130,12 +2978,11 @@
       <c r="H54" s="13"/>
       <c r="I54" s="1"/>
       <c r="J54" s="8"/>
-      <c r="K54" s="28"/>
-      <c r="L54" s="28"/>
-      <c r="M54" s="43"/>
-      <c r="N54" s="34"/>
-    </row>
-    <row r="55" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K54" s="26"/>
+      <c r="L54" s="26"/>
+      <c r="M54" s="34"/>
+    </row>
+    <row r="55" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="3"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -3146,12 +2993,11 @@
       <c r="H55" s="13"/>
       <c r="I55" s="1"/>
       <c r="J55" s="8"/>
-      <c r="K55" s="28"/>
-      <c r="L55" s="28"/>
-      <c r="M55" s="43"/>
-      <c r="N55" s="34"/>
-    </row>
-    <row r="56" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K55" s="26"/>
+      <c r="L55" s="26"/>
+      <c r="M55" s="34"/>
+    </row>
+    <row r="56" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="3"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -3162,12 +3008,11 @@
       <c r="H56" s="13"/>
       <c r="I56" s="1"/>
       <c r="J56" s="8"/>
-      <c r="K56" s="28"/>
-      <c r="L56" s="28"/>
-      <c r="M56" s="43"/>
-      <c r="N56" s="34"/>
-    </row>
-    <row r="57" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K56" s="26"/>
+      <c r="L56" s="26"/>
+      <c r="M56" s="34"/>
+    </row>
+    <row r="57" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="3"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -3178,12 +3023,11 @@
       <c r="H57" s="13"/>
       <c r="I57" s="1"/>
       <c r="J57" s="8"/>
-      <c r="K57" s="28"/>
-      <c r="L57" s="28"/>
-      <c r="M57" s="43"/>
-      <c r="N57" s="34"/>
-    </row>
-    <row r="58" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K57" s="26"/>
+      <c r="L57" s="26"/>
+      <c r="M57" s="34"/>
+    </row>
+    <row r="58" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="3"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -3194,12 +3038,11 @@
       <c r="H58" s="13"/>
       <c r="I58" s="1"/>
       <c r="J58" s="8"/>
-      <c r="K58" s="28"/>
-      <c r="L58" s="28"/>
-      <c r="M58" s="43"/>
-      <c r="N58" s="34"/>
-    </row>
-    <row r="59" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K58" s="26"/>
+      <c r="L58" s="26"/>
+      <c r="M58" s="34"/>
+    </row>
+    <row r="59" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="3"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -3210,12 +3053,11 @@
       <c r="H59" s="13"/>
       <c r="I59" s="1"/>
       <c r="J59" s="8"/>
-      <c r="K59" s="28"/>
-      <c r="L59" s="28"/>
-      <c r="M59" s="43"/>
-      <c r="N59" s="34"/>
-    </row>
-    <row r="60" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K59" s="26"/>
+      <c r="L59" s="26"/>
+      <c r="M59" s="34"/>
+    </row>
+    <row r="60" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="3"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -3226,12 +3068,11 @@
       <c r="H60" s="13"/>
       <c r="I60" s="1"/>
       <c r="J60" s="8"/>
-      <c r="K60" s="28"/>
-      <c r="L60" s="28"/>
-      <c r="M60" s="43"/>
-      <c r="N60" s="34"/>
-    </row>
-    <row r="61" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K60" s="26"/>
+      <c r="L60" s="26"/>
+      <c r="M60" s="34"/>
+    </row>
+    <row r="61" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="3"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -3242,12 +3083,11 @@
       <c r="H61" s="13"/>
       <c r="I61" s="1"/>
       <c r="J61" s="8"/>
-      <c r="K61" s="28"/>
-      <c r="L61" s="28"/>
-      <c r="M61" s="43"/>
-      <c r="N61" s="34"/>
-    </row>
-    <row r="62" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K61" s="26"/>
+      <c r="L61" s="26"/>
+      <c r="M61" s="34"/>
+    </row>
+    <row r="62" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="3"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -3258,12 +3098,11 @@
       <c r="H62" s="13"/>
       <c r="I62" s="1"/>
       <c r="J62" s="8"/>
-      <c r="K62" s="28"/>
-      <c r="L62" s="28"/>
-      <c r="M62" s="43"/>
-      <c r="N62" s="34"/>
-    </row>
-    <row r="63" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K62" s="26"/>
+      <c r="L62" s="26"/>
+      <c r="M62" s="34"/>
+    </row>
+    <row r="63" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="3"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -3274,12 +3113,11 @@
       <c r="H63" s="13"/>
       <c r="I63" s="1"/>
       <c r="J63" s="8"/>
-      <c r="K63" s="28"/>
-      <c r="L63" s="28"/>
-      <c r="M63" s="43"/>
-      <c r="N63" s="34"/>
-    </row>
-    <row r="64" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K63" s="26"/>
+      <c r="L63" s="26"/>
+      <c r="M63" s="34"/>
+    </row>
+    <row r="64" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="3"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -3290,12 +3128,11 @@
       <c r="H64" s="13"/>
       <c r="I64" s="1"/>
       <c r="J64" s="8"/>
-      <c r="K64" s="28"/>
-      <c r="L64" s="28"/>
-      <c r="M64" s="43"/>
-      <c r="N64" s="34"/>
-    </row>
-    <row r="65" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K64" s="26"/>
+      <c r="L64" s="26"/>
+      <c r="M64" s="34"/>
+    </row>
+    <row r="65" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="3"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -3306,12 +3143,11 @@
       <c r="H65" s="13"/>
       <c r="I65" s="1"/>
       <c r="J65" s="8"/>
-      <c r="K65" s="28"/>
-      <c r="L65" s="28"/>
-      <c r="M65" s="43"/>
-      <c r="N65" s="34"/>
-    </row>
-    <row r="66" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K65" s="26"/>
+      <c r="L65" s="26"/>
+      <c r="M65" s="34"/>
+    </row>
+    <row r="66" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="3"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -3322,12 +3158,11 @@
       <c r="H66" s="13"/>
       <c r="I66" s="1"/>
       <c r="J66" s="8"/>
-      <c r="K66" s="28"/>
-      <c r="L66" s="28"/>
-      <c r="M66" s="43"/>
-      <c r="N66" s="34"/>
-    </row>
-    <row r="67" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K66" s="26"/>
+      <c r="L66" s="26"/>
+      <c r="M66" s="34"/>
+    </row>
+    <row r="67" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="3"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -3338,12 +3173,11 @@
       <c r="H67" s="13"/>
       <c r="I67" s="1"/>
       <c r="J67" s="8"/>
-      <c r="K67" s="28"/>
-      <c r="L67" s="28"/>
-      <c r="M67" s="43"/>
-      <c r="N67" s="34"/>
-    </row>
-    <row r="68" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K67" s="26"/>
+      <c r="L67" s="26"/>
+      <c r="M67" s="34"/>
+    </row>
+    <row r="68" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="3"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -3354,12 +3188,11 @@
       <c r="H68" s="13"/>
       <c r="I68" s="1"/>
       <c r="J68" s="8"/>
-      <c r="K68" s="28"/>
-      <c r="L68" s="28"/>
-      <c r="M68" s="43"/>
-      <c r="N68" s="34"/>
-    </row>
-    <row r="69" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K68" s="26"/>
+      <c r="L68" s="26"/>
+      <c r="M68" s="34"/>
+    </row>
+    <row r="69" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="3"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -3370,12 +3203,11 @@
       <c r="H69" s="13"/>
       <c r="I69" s="1"/>
       <c r="J69" s="8"/>
-      <c r="K69" s="28"/>
-      <c r="L69" s="28"/>
-      <c r="M69" s="43"/>
-      <c r="N69" s="34"/>
-    </row>
-    <row r="70" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K69" s="26"/>
+      <c r="L69" s="26"/>
+      <c r="M69" s="34"/>
+    </row>
+    <row r="70" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="3"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -3386,12 +3218,11 @@
       <c r="H70" s="13"/>
       <c r="I70" s="1"/>
       <c r="J70" s="8"/>
-      <c r="K70" s="28"/>
-      <c r="L70" s="28"/>
-      <c r="M70" s="43"/>
-      <c r="N70" s="34"/>
-    </row>
-    <row r="71" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K70" s="26"/>
+      <c r="L70" s="26"/>
+      <c r="M70" s="34"/>
+    </row>
+    <row r="71" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="3"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -3402,12 +3233,11 @@
       <c r="H71" s="13"/>
       <c r="I71" s="1"/>
       <c r="J71" s="8"/>
-      <c r="K71" s="28"/>
-      <c r="L71" s="28"/>
-      <c r="M71" s="43"/>
-      <c r="N71" s="34"/>
-    </row>
-    <row r="72" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K71" s="26"/>
+      <c r="L71" s="26"/>
+      <c r="M71" s="34"/>
+    </row>
+    <row r="72" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="3"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -3418,12 +3248,11 @@
       <c r="H72" s="13"/>
       <c r="I72" s="1"/>
       <c r="J72" s="8"/>
-      <c r="K72" s="28"/>
-      <c r="L72" s="28"/>
-      <c r="M72" s="43"/>
-      <c r="N72" s="34"/>
-    </row>
-    <row r="73" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K72" s="26"/>
+      <c r="L72" s="26"/>
+      <c r="M72" s="34"/>
+    </row>
+    <row r="73" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="3"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -3434,12 +3263,11 @@
       <c r="H73" s="13"/>
       <c r="I73" s="1"/>
       <c r="J73" s="8"/>
-      <c r="K73" s="28"/>
-      <c r="L73" s="28"/>
-      <c r="M73" s="43"/>
-      <c r="N73" s="34"/>
-    </row>
-    <row r="74" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K73" s="26"/>
+      <c r="L73" s="26"/>
+      <c r="M73" s="34"/>
+    </row>
+    <row r="74" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="3"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -3450,12 +3278,11 @@
       <c r="H74" s="13"/>
       <c r="I74" s="1"/>
       <c r="J74" s="8"/>
-      <c r="K74" s="28"/>
-      <c r="L74" s="28"/>
-      <c r="M74" s="43"/>
-      <c r="N74" s="34"/>
-    </row>
-    <row r="75" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K74" s="26"/>
+      <c r="L74" s="26"/>
+      <c r="M74" s="34"/>
+    </row>
+    <row r="75" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="3"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -3466,12 +3293,11 @@
       <c r="H75" s="13"/>
       <c r="I75" s="1"/>
       <c r="J75" s="8"/>
-      <c r="K75" s="28"/>
-      <c r="L75" s="28"/>
-      <c r="M75" s="43"/>
-      <c r="N75" s="34"/>
-    </row>
-    <row r="76" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K75" s="26"/>
+      <c r="L75" s="26"/>
+      <c r="M75" s="34"/>
+    </row>
+    <row r="76" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="3"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -3482,12 +3308,11 @@
       <c r="H76" s="13"/>
       <c r="I76" s="1"/>
       <c r="J76" s="8"/>
-      <c r="K76" s="28"/>
-      <c r="L76" s="28"/>
-      <c r="M76" s="43"/>
-      <c r="N76" s="34"/>
-    </row>
-    <row r="77" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K76" s="26"/>
+      <c r="L76" s="26"/>
+      <c r="M76" s="34"/>
+    </row>
+    <row r="77" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="3"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -3498,12 +3323,11 @@
       <c r="H77" s="13"/>
       <c r="I77" s="1"/>
       <c r="J77" s="8"/>
-      <c r="K77" s="28"/>
-      <c r="L77" s="28"/>
-      <c r="M77" s="43"/>
-      <c r="N77" s="34"/>
-    </row>
-    <row r="78" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K77" s="26"/>
+      <c r="L77" s="26"/>
+      <c r="M77" s="34"/>
+    </row>
+    <row r="78" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="3"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -3514,12 +3338,11 @@
       <c r="H78" s="13"/>
       <c r="I78" s="1"/>
       <c r="J78" s="8"/>
-      <c r="K78" s="28"/>
-      <c r="L78" s="28"/>
-      <c r="M78" s="43"/>
-      <c r="N78" s="34"/>
-    </row>
-    <row r="79" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K78" s="26"/>
+      <c r="L78" s="26"/>
+      <c r="M78" s="34"/>
+    </row>
+    <row r="79" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="3"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -3530,12 +3353,11 @@
       <c r="H79" s="13"/>
       <c r="I79" s="1"/>
       <c r="J79" s="8"/>
-      <c r="K79" s="28"/>
-      <c r="L79" s="28"/>
-      <c r="M79" s="43"/>
-      <c r="N79" s="34"/>
-    </row>
-    <row r="80" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K79" s="26"/>
+      <c r="L79" s="26"/>
+      <c r="M79" s="34"/>
+    </row>
+    <row r="80" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="3"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -3546,12 +3368,11 @@
       <c r="H80" s="13"/>
       <c r="I80" s="1"/>
       <c r="J80" s="8"/>
-      <c r="K80" s="28"/>
-      <c r="L80" s="28"/>
-      <c r="M80" s="43"/>
-      <c r="N80" s="34"/>
-    </row>
-    <row r="81" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K80" s="26"/>
+      <c r="L80" s="26"/>
+      <c r="M80" s="34"/>
+    </row>
+    <row r="81" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="3"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -3562,12 +3383,11 @@
       <c r="H81" s="13"/>
       <c r="I81" s="1"/>
       <c r="J81" s="8"/>
-      <c r="K81" s="28"/>
-      <c r="L81" s="28"/>
-      <c r="M81" s="43"/>
-      <c r="N81" s="34"/>
-    </row>
-    <row r="82" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K81" s="26"/>
+      <c r="L81" s="26"/>
+      <c r="M81" s="34"/>
+    </row>
+    <row r="82" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="3"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -3578,12 +3398,11 @@
       <c r="H82" s="13"/>
       <c r="I82" s="1"/>
       <c r="J82" s="8"/>
-      <c r="K82" s="28"/>
-      <c r="L82" s="28"/>
-      <c r="M82" s="43"/>
-      <c r="N82" s="34"/>
-    </row>
-    <row r="83" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K82" s="26"/>
+      <c r="L82" s="26"/>
+      <c r="M82" s="34"/>
+    </row>
+    <row r="83" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="3"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -3594,12 +3413,11 @@
       <c r="H83" s="13"/>
       <c r="I83" s="1"/>
       <c r="J83" s="8"/>
-      <c r="K83" s="28"/>
-      <c r="L83" s="28"/>
-      <c r="M83" s="43"/>
-      <c r="N83" s="34"/>
-    </row>
-    <row r="84" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K83" s="26"/>
+      <c r="L83" s="26"/>
+      <c r="M83" s="34"/>
+    </row>
+    <row r="84" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="3"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -3610,12 +3428,11 @@
       <c r="H84" s="13"/>
       <c r="I84" s="1"/>
       <c r="J84" s="8"/>
-      <c r="K84" s="28"/>
-      <c r="L84" s="28"/>
-      <c r="M84" s="43"/>
-      <c r="N84" s="34"/>
-    </row>
-    <row r="85" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K84" s="26"/>
+      <c r="L84" s="26"/>
+      <c r="M84" s="34"/>
+    </row>
+    <row r="85" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="3"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -3626,12 +3443,11 @@
       <c r="H85" s="13"/>
       <c r="I85" s="1"/>
       <c r="J85" s="8"/>
-      <c r="K85" s="28"/>
-      <c r="L85" s="28"/>
-      <c r="M85" s="43"/>
-      <c r="N85" s="34"/>
-    </row>
-    <row r="86" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K85" s="26"/>
+      <c r="L85" s="26"/>
+      <c r="M85" s="34"/>
+    </row>
+    <row r="86" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="3"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -3642,12 +3458,11 @@
       <c r="H86" s="13"/>
       <c r="I86" s="1"/>
       <c r="J86" s="8"/>
-      <c r="K86" s="28"/>
-      <c r="L86" s="28"/>
-      <c r="M86" s="43"/>
-      <c r="N86" s="34"/>
-    </row>
-    <row r="87" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K86" s="26"/>
+      <c r="L86" s="26"/>
+      <c r="M86" s="34"/>
+    </row>
+    <row r="87" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="3"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -3658,12 +3473,11 @@
       <c r="H87" s="13"/>
       <c r="I87" s="1"/>
       <c r="J87" s="8"/>
-      <c r="K87" s="28"/>
-      <c r="L87" s="28"/>
-      <c r="M87" s="43"/>
-      <c r="N87" s="34"/>
-    </row>
-    <row r="88" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K87" s="26"/>
+      <c r="L87" s="26"/>
+      <c r="M87" s="34"/>
+    </row>
+    <row r="88" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="3"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -3674,12 +3488,11 @@
       <c r="H88" s="13"/>
       <c r="I88" s="1"/>
       <c r="J88" s="8"/>
-      <c r="K88" s="28"/>
-      <c r="L88" s="28"/>
-      <c r="M88" s="43"/>
-      <c r="N88" s="34"/>
-    </row>
-    <row r="89" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K88" s="26"/>
+      <c r="L88" s="26"/>
+      <c r="M88" s="34"/>
+    </row>
+    <row r="89" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="3"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -3690,12 +3503,11 @@
       <c r="H89" s="13"/>
       <c r="I89" s="1"/>
       <c r="J89" s="8"/>
-      <c r="K89" s="28"/>
-      <c r="L89" s="28"/>
-      <c r="M89" s="43"/>
-      <c r="N89" s="34"/>
-    </row>
-    <row r="90" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K89" s="26"/>
+      <c r="L89" s="26"/>
+      <c r="M89" s="34"/>
+    </row>
+    <row r="90" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="3"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -3706,12 +3518,11 @@
       <c r="H90" s="13"/>
       <c r="I90" s="1"/>
       <c r="J90" s="8"/>
-      <c r="K90" s="28"/>
-      <c r="L90" s="28"/>
-      <c r="M90" s="43"/>
-      <c r="N90" s="34"/>
-    </row>
-    <row r="91" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K90" s="26"/>
+      <c r="L90" s="26"/>
+      <c r="M90" s="34"/>
+    </row>
+    <row r="91" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="3"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -3722,12 +3533,11 @@
       <c r="H91" s="13"/>
       <c r="I91" s="1"/>
       <c r="J91" s="8"/>
-      <c r="K91" s="28"/>
-      <c r="L91" s="28"/>
-      <c r="M91" s="43"/>
-      <c r="N91" s="34"/>
-    </row>
-    <row r="92" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K91" s="26"/>
+      <c r="L91" s="26"/>
+      <c r="M91" s="34"/>
+    </row>
+    <row r="92" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="3"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -3738,12 +3548,11 @@
       <c r="H92" s="13"/>
       <c r="I92" s="1"/>
       <c r="J92" s="8"/>
-      <c r="K92" s="28"/>
-      <c r="L92" s="28"/>
-      <c r="M92" s="43"/>
-      <c r="N92" s="34"/>
-    </row>
-    <row r="93" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K92" s="26"/>
+      <c r="L92" s="26"/>
+      <c r="M92" s="34"/>
+    </row>
+    <row r="93" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="3"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -3754,12 +3563,11 @@
       <c r="H93" s="13"/>
       <c r="I93" s="1"/>
       <c r="J93" s="8"/>
-      <c r="K93" s="28"/>
-      <c r="L93" s="28"/>
-      <c r="M93" s="43"/>
-      <c r="N93" s="34"/>
-    </row>
-    <row r="94" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K93" s="26"/>
+      <c r="L93" s="26"/>
+      <c r="M93" s="34"/>
+    </row>
+    <row r="94" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="3"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -3770,12 +3578,11 @@
       <c r="H94" s="13"/>
       <c r="I94" s="1"/>
       <c r="J94" s="8"/>
-      <c r="K94" s="28"/>
-      <c r="L94" s="28"/>
-      <c r="M94" s="43"/>
-      <c r="N94" s="34"/>
-    </row>
-    <row r="95" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K94" s="26"/>
+      <c r="L94" s="26"/>
+      <c r="M94" s="34"/>
+    </row>
+    <row r="95" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="3"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -3786,12 +3593,11 @@
       <c r="H95" s="13"/>
       <c r="I95" s="1"/>
       <c r="J95" s="8"/>
-      <c r="K95" s="28"/>
-      <c r="L95" s="28"/>
-      <c r="M95" s="43"/>
-      <c r="N95" s="34"/>
-    </row>
-    <row r="96" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K95" s="26"/>
+      <c r="L95" s="26"/>
+      <c r="M95" s="34"/>
+    </row>
+    <row r="96" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="3"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -3802,12 +3608,11 @@
       <c r="H96" s="13"/>
       <c r="I96" s="1"/>
       <c r="J96" s="8"/>
-      <c r="K96" s="28"/>
-      <c r="L96" s="28"/>
-      <c r="M96" s="43"/>
-      <c r="N96" s="34"/>
-    </row>
-    <row r="97" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K96" s="26"/>
+      <c r="L96" s="26"/>
+      <c r="M96" s="34"/>
+    </row>
+    <row r="97" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="3"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -3818,12 +3623,11 @@
       <c r="H97" s="13"/>
       <c r="I97" s="1"/>
       <c r="J97" s="8"/>
-      <c r="K97" s="28"/>
-      <c r="L97" s="28"/>
-      <c r="M97" s="43"/>
-      <c r="N97" s="34"/>
-    </row>
-    <row r="98" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K97" s="26"/>
+      <c r="L97" s="26"/>
+      <c r="M97" s="34"/>
+    </row>
+    <row r="98" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="3"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -3836,10 +3640,9 @@
       <c r="J98" s="8"/>
       <c r="K98" s="8"/>
       <c r="L98" s="8"/>
-      <c r="M98" s="43"/>
-      <c r="N98" s="34"/>
-    </row>
-    <row r="99" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M98" s="34"/>
+    </row>
+    <row r="99" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="3"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -3852,10 +3655,9 @@
       <c r="J99" s="8"/>
       <c r="K99" s="8"/>
       <c r="L99" s="8"/>
-      <c r="M99" s="43"/>
-      <c r="N99" s="34"/>
-    </row>
-    <row r="100" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M99" s="34"/>
+    </row>
+    <row r="100" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="3"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -3868,10 +3670,9 @@
       <c r="J100" s="8"/>
       <c r="K100" s="8"/>
       <c r="L100" s="8"/>
-      <c r="M100" s="43"/>
-      <c r="N100" s="34"/>
-    </row>
-    <row r="101" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M100" s="34"/>
+    </row>
+    <row r="101" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A101" s="4"/>
       <c r="B101" s="5"/>
       <c r="C101" s="5"/>
@@ -3884,15 +3685,36 @@
       <c r="J101" s="10"/>
       <c r="K101" s="10"/>
       <c r="L101" s="10"/>
-      <c r="M101" s="41"/>
-      <c r="N101" s="34"/>
-    </row>
-    <row r="102" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M101" s="33"/>
+    </row>
+    <row r="102" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="K102" s="11"/>
       <c r="L102" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="A8:M8"/>
+    <mergeCell ref="A9:M9"/>
+    <mergeCell ref="A10:M10"/>
+    <mergeCell ref="A11:M11"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:H15"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="F14:I14"/>
     <mergeCell ref="A12:M12"/>
@@ -3909,28 +3731,6 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="M14:M16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="A8:M8"/>
-    <mergeCell ref="A9:M9"/>
-    <mergeCell ref="A10:M10"/>
-    <mergeCell ref="A11:M11"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F17:F1048576 F1:F3 F7 F13">

</xml_diff>